<commit_message>
Hopefully fix cxn errors
</commit_message>
<xml_diff>
--- a/AlexTorda/DataAnalysis_AlexTorda.xlsx
+++ b/AlexTorda/DataAnalysis_AlexTorda.xlsx
@@ -1,30 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GENIE2K\CAMFILES\AlexTorda\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stlgo\Documents\Github\phy417s-mw\AlexTorda\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6ECB44B-547E-40FE-8219-5D628173D391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>Angle</t>
   </si>
@@ -104,19 +116,37 @@
     <t>barns</t>
   </si>
   <si>
-    <t>N (counts per second)</t>
-  </si>
-  <si>
     <t>C</t>
   </si>
   <si>
     <t>cxn error</t>
   </si>
+  <si>
+    <t>cxn</t>
+  </si>
+  <si>
+    <t>new attempt for cxn error</t>
+  </si>
+  <si>
+    <t>dC^2</t>
+  </si>
+  <si>
+    <t>C (counts per second)</t>
+  </si>
+  <si>
+    <t>total cxn err</t>
+  </si>
+  <si>
+    <t>% of total error</t>
+  </si>
+  <si>
+    <t>other error</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -210,7 +240,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -555,7 +584,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -673,7 +701,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -804,7 +831,35 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Cross</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Section</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -866,100 +921,11 @@
             </c:spPr>
           </c:marker>
           <c:errBars>
-            <c:errDir val="y"/>
+            <c:errDir val="x"/>
             <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
+            <c:errValType val="fixedVal"/>
             <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>Sheet1!$K$25:$K$36</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="12"/>
-                  <c:pt idx="0">
-                    <c:v>3.0407681286844026</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>3.6349221155018201</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>4.5170534523730943</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>2.5582209529663267</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>3.4966276634297007</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>3.0112490023668461</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>2.1533170094719414</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>2.3467046124862398</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>1.6979180298760712</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>2.2556792257075888</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>3.14112718583225</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>3.7691773819009606</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>Sheet1!$K$25:$K$36</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="12"/>
-                  <c:pt idx="0">
-                    <c:v>3.0407681286844026</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>3.6349221155018201</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>4.5170534523730943</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>2.5582209529663267</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>3.4966276634297007</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>3.0112490023668461</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>2.1533170094719414</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>2.3467046124862398</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>1.6979180298760712</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>2.2556792257075888</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>3.14112718583225</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>3.7691773819009606</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
+            <c:val val="1"/>
             <c:spPr>
               <a:noFill/>
               <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -975,11 +941,100 @@
             </c:spPr>
           </c:errBars>
           <c:errBars>
-            <c:errDir val="x"/>
+            <c:errDir val="y"/>
             <c:errBarType val="both"/>
-            <c:errValType val="fixedVal"/>
+            <c:errValType val="cust"/>
             <c:noEndCap val="0"/>
-            <c:val val="1"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$L$25:$L$36</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="12"/>
+                  <c:pt idx="0">
+                    <c:v>0.13864361043291312</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.22296588944999363</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.19706271721777735</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.19225556943928462</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.1886249881086236</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.23177695429664308</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.17772508403410603</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0.12986303721844897</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>0.13507038428660223</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>0.17658449624656516</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>0.21784691183748625</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>0.23009019627604299</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$L$25:$L$36</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="12"/>
+                  <c:pt idx="0">
+                    <c:v>0.13864361043291312</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.22296588944999363</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.19706271721777735</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.19225556943928462</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.1886249881086236</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.23177695429664308</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.17772508403410603</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0.12986303721844897</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>0.13507038428660223</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>0.17658449624656516</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>0.21784691183748625</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>0.23009019627604299</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
             <c:spPr>
               <a:noFill/>
               <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -1046,40 +1101,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>8.8468372461033304</c:v>
+                  <c:v>1.4904080857349506</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.683957826907454</c:v>
+                  <c:v>1.4629681321542212</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.4743062966202034</c:v>
+                  <c:v>1.2591806800389616</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.8666502748814837</c:v>
+                  <c:v>0.81987434812620341</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.2751612992158057</c:v>
+                  <c:v>0.88869534221060509</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.5985787343404514</c:v>
+                  <c:v>0.77471289884626338</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.4815172498278648</c:v>
+                  <c:v>0.58652389723283871</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.9183468599842191</c:v>
+                  <c:v>0.66011566398001587</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.9556034951330274</c:v>
+                  <c:v>0.49792431180001562</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.8984545283692427</c:v>
+                  <c:v>0.99370024313418637</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8.4641849857139277</c:v>
+                  <c:v>1.4259434632891927</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7.3774606491882659</c:v>
+                  <c:v>1.2428652972659406</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1123,6 +1178,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Angle</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (Degrees)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1185,6 +1300,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Cross Section in Barns^-2</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1236,6 +1406,629 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Error</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Contributions</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Counting Rate Error</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$25:$D$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$R$26:$R$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>39.383410159699096</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>39.376395751965006</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>39.357670839589197</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>39.369923294033882</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>39.357259652027373</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>39.366435210210497</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>39.370226996614868</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>39.379525623080269</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>39.380794645334262</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>39.377381749086815</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>39.379752422023998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>39.373487612387983</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9E1C-4272-B686-B609482C07F9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Other Errors</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$25:$D$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$S$26:$S$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>60.616589840300904</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60.623604248034994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60.642329160410803</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60.630076705966118</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60.642740347972627</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60.633564789789503</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60.629773003385132</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>60.620474376919731</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>60.619205354665738</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>60.622618250913185</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>60.620247577976002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60.626512387612017</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9E1C-4272-B686-B609482C07F9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1155826736"/>
+        <c:axId val="1182766528"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1155826736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Angle</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (Degrees)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1182766528"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1182766528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Percentage</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1155826736"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -1351,6 +2144,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2383,24 +3216,533 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>295276</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>180976</xdr:rowOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>228601</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>142876</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2417,20 +3759,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>366712</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>357187</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>61911</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>404812</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2445,18 +3793,54 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>252412</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>23812</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A338D0AF-BA95-C8AC-2934-E15FDE302136}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="D24:F36" totalsRowShown="0">
-  <autoFilter ref="D24:F36"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table4" displayName="Table4" ref="D24:F36" totalsRowShown="0">
+  <autoFilter ref="D24:F36" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Angle"/>
-    <tableColumn id="2" name="Energy">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Angle"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Energy">
       <calculatedColumnFormula>0.0000978*(D7)-0.0247</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="EnergyErr">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="EnergyErr">
       <calculatedColumnFormula>0.0000978*(E7)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2726,19 +4110,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:T36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A3:T37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O39" sqref="O39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="9" width="11.5703125" customWidth="1"/>
-    <col min="10" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -2797,10 +4182,10 @@
         <v>8</v>
       </c>
       <c r="Q6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R6" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -2826,7 +4211,7 @@
         <v>0.13348450001396303</v>
       </c>
       <c r="H7">
-        <f>SQRT((E7*F7)^2 +(G7*B7)^2)</f>
+        <f t="shared" ref="H7:H18" si="0">SQRT((E7*F7)^2 +(G7*B7)^2)</f>
         <v>1.8733738819372556</v>
       </c>
       <c r="J7">
@@ -2857,7 +4242,7 @@
         <v>20</v>
       </c>
       <c r="B8">
-        <f t="shared" ref="B8:B18" si="0">PI()*A8/180</f>
+        <f t="shared" ref="B8:B18" si="1">PI()*A8/180</f>
         <v>0.3490658503988659</v>
       </c>
       <c r="D8">
@@ -2867,15 +4252,15 @@
         <v>21.554400000000001</v>
       </c>
       <c r="F8">
-        <f t="shared" ref="F8:F18" si="1">-E26*(1+COS(B8)/$C$4)^-2 +(1+E26*(1+COS(B8))/$C$4)^-1</f>
+        <f t="shared" ref="F8:F18" si="2">-E26*(1+COS(B8)/$C$4)^-2 +(1+E26*(1+COS(B8))/$C$4)^-1</f>
         <v>0.23336400907564081</v>
       </c>
       <c r="G8">
-        <f t="shared" ref="G8:G18" si="2">-E26*(-E26*SIN(B8)/$C$4)</f>
+        <f t="shared" ref="G8:G18" si="3">-E26*(-E26*SIN(B8)/$C$4)</f>
         <v>0.2364513600978394</v>
       </c>
       <c r="H8">
-        <f>SQRT((E8*F8)^2 +(G8*B8)^2)</f>
+        <f t="shared" si="0"/>
         <v>5.0306983229516389</v>
       </c>
       <c r="J8">
@@ -2894,7 +4279,7 @@
         <v>2000</v>
       </c>
       <c r="R8">
-        <f t="shared" ref="R8:R18" si="3">J8*M8*SQRT(2*PI())/(P8*(16384/200))</f>
+        <f t="shared" ref="R8:R18" si="4">J8*M8*SQRT(2*PI())/(P8*(16384/200))</f>
         <v>4.796393651898657</v>
       </c>
       <c r="T8" t="s">
@@ -2906,7 +4291,7 @@
         <v>30</v>
       </c>
       <c r="B9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.52359877559829882</v>
       </c>
       <c r="D9">
@@ -2916,15 +4301,15 @@
         <v>32.943300000000001</v>
       </c>
       <c r="F9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26291997301747122</v>
       </c>
       <c r="G9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.28379344168331178</v>
       </c>
       <c r="H9">
-        <f>SQRT((E9*F9)^2 +(G9*B9)^2)</f>
+        <f t="shared" si="0"/>
         <v>8.6627260749472228</v>
       </c>
       <c r="J9">
@@ -2943,7 +4328,7 @@
         <v>2600</v>
       </c>
       <c r="R9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.2062139826334768</v>
       </c>
       <c r="T9" t="s">
@@ -2955,7 +4340,7 @@
         <v>40</v>
       </c>
       <c r="B10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.69813170079773179</v>
       </c>
       <c r="D10">
@@ -2965,15 +4350,15 @@
         <v>34.072400000000002</v>
       </c>
       <c r="F10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.30025169572630073</v>
       </c>
       <c r="G10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.28794314816533656</v>
       </c>
       <c r="H10">
-        <f>SQRT((E10*F10)^2 +(G10*B10)^2)</f>
+        <f t="shared" si="0"/>
         <v>10.232270700159976</v>
       </c>
       <c r="J10">
@@ -2992,7 +4377,7 @@
         <v>3000</v>
       </c>
       <c r="R10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.653030573318822</v>
       </c>
     </row>
@@ -3001,7 +4386,7 @@
         <v>50</v>
       </c>
       <c r="B11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.87266462599716477</v>
       </c>
       <c r="D11">
@@ -3011,15 +4396,15 @@
         <v>36.585700000000003</v>
       </c>
       <c r="F11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.333617233650981</v>
       </c>
       <c r="G11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.28021896979766842</v>
       </c>
       <c r="H11">
-        <f>SQRT((E11*F11)^2 +(G11*B11)^2)</f>
+        <f t="shared" si="0"/>
         <v>12.208069406454195</v>
       </c>
       <c r="J11">
@@ -3038,7 +4423,7 @@
         <v>3500</v>
       </c>
       <c r="R11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.8668840725038938</v>
       </c>
       <c r="T11" t="s">
@@ -3050,7 +4435,7 @@
         <v>60</v>
       </c>
       <c r="B12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.0471975511965976</v>
       </c>
       <c r="D12">
@@ -3060,15 +4445,15 @@
         <v>39.036900000000003</v>
       </c>
       <c r="F12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.36654006212307016</v>
       </c>
       <c r="G12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.25787393854044227</v>
       </c>
       <c r="H12">
-        <f>SQRT((E12*F12)^2 +(G12*B12)^2)</f>
+        <f t="shared" si="0"/>
         <v>14.311135793831324</v>
       </c>
       <c r="J12">
@@ -3087,7 +4472,7 @@
         <v>4000</v>
       </c>
       <c r="R12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.3412927259547827</v>
       </c>
     </row>
@@ -3096,7 +4481,7 @@
         <v>70</v>
       </c>
       <c r="B13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.2217304763960306</v>
       </c>
       <c r="D13">
@@ -3106,15 +4491,15 @@
         <v>31.535699999999999</v>
       </c>
       <c r="F13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.40411998528880649</v>
       </c>
       <c r="G13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.21505417955429024</v>
       </c>
       <c r="H13">
-        <f>SQRT((E13*F13)^2 +(G13*B13)^2)</f>
+        <f t="shared" si="0"/>
         <v>12.746914676132539</v>
       </c>
       <c r="J13">
@@ -3133,7 +4518,7 @@
         <v>6000</v>
       </c>
       <c r="R13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.6893996926660979</v>
       </c>
     </row>
@@ -3142,7 +4527,7 @@
         <v>80</v>
       </c>
       <c r="B14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.3962634015954636</v>
       </c>
       <c r="D14">
@@ -3152,15 +4537,15 @@
         <v>12.6167</v>
       </c>
       <c r="F14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.41692348057297268</v>
       </c>
       <c r="G14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.18035069088279143</v>
       </c>
       <c r="H14">
-        <f>SQRT((E14*F14)^2 +(G14*B14)^2)</f>
+        <f t="shared" si="0"/>
         <v>5.2662225415727733</v>
       </c>
       <c r="J14">
@@ -3179,7 +4564,7 @@
         <v>20000</v>
       </c>
       <c r="R14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.881115527372369</v>
       </c>
     </row>
@@ -3188,7 +4573,7 @@
         <v>90</v>
       </c>
       <c r="B15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5707963267948966</v>
       </c>
       <c r="D15">
@@ -3198,15 +4583,15 @@
         <v>14.2506</v>
       </c>
       <c r="F15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.38083195244710444</v>
       </c>
       <c r="G15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.14465866488824292</v>
       </c>
       <c r="H15">
-        <f>SQRT((E15*F15)^2 +(G15*B15)^2)</f>
+        <f t="shared" si="0"/>
         <v>5.431838727408711</v>
       </c>
       <c r="J15">
@@ -3225,7 +4610,7 @@
         <v>20000</v>
       </c>
       <c r="R15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3184175257970636</v>
       </c>
     </row>
@@ -3234,7 +4619,7 @@
         <v>-10</v>
       </c>
       <c r="B16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.17453292519943295</v>
       </c>
       <c r="D16">
@@ -3244,15 +4629,15 @@
         <v>25.226500000000001</v>
       </c>
       <c r="F16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.21745690064627096</v>
       </c>
       <c r="G16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-0.1340320431488789</v>
       </c>
       <c r="H16">
-        <f>SQRT((E16*F16)^2 +(G16*B16)^2)</f>
+        <f t="shared" si="0"/>
         <v>5.4857263822469653</v>
       </c>
       <c r="J16">
@@ -3271,16 +4656,16 @@
         <v>2000</v>
       </c>
       <c r="R16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.3423990752253254</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>-20</v>
       </c>
       <c r="B17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.3490658503988659</v>
       </c>
       <c r="D17">
@@ -3290,15 +4675,15 @@
         <v>18.1159</v>
       </c>
       <c r="F17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.23430716622938946</v>
       </c>
       <c r="G17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-0.23489997686514733</v>
       </c>
       <c r="H17">
-        <f>SQRT((E17*F17)^2 +(G17*B17)^2)</f>
+        <f t="shared" si="0"/>
         <v>4.2454770823753014</v>
       </c>
       <c r="J17">
@@ -3317,16 +4702,16 @@
         <v>2000</v>
       </c>
       <c r="R17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.6596450879694302</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>-30</v>
       </c>
       <c r="B18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.52359877559829882</v>
       </c>
       <c r="D18">
@@ -3336,15 +4721,15 @@
         <v>27.087399999999999</v>
       </c>
       <c r="F18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.2597758700818914</v>
       </c>
       <c r="G18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-0.28985315279871482</v>
       </c>
       <c r="H18">
-        <f>SQRT((E18*F18)^2 +(G18*B18)^2)</f>
+        <f t="shared" si="0"/>
         <v>7.0382893680995604</v>
       </c>
       <c r="J18">
@@ -3363,11 +4748,11 @@
         <v>2600</v>
       </c>
       <c r="R18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.9635640852271412</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="I22" t="s">
         <v>23</v>
       </c>
@@ -3378,21 +4763,20 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="I23">
-        <f>(((922500/200)+(793300/200))/2)/0.38</f>
-        <v>11288.157894736842</v>
+        <v>10469.5</v>
       </c>
       <c r="K23">
-        <f>(100^3)*2.7*(6.022E+23)*13/27</f>
-        <v>7.828600000000001E+29</v>
+        <f>2.7*(6.022E+23)*13/27</f>
+        <v>7.8286000000000012E+23</v>
       </c>
       <c r="L23">
-        <f>4*PI()*(0.5/(36))^2</f>
-        <v>2.4240684055476798E-3</v>
+        <f>4*PI()*(4/(36))^2</f>
+        <v>0.15514037795505151</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
         <v>0</v>
       </c>
@@ -3405,14 +4789,23 @@
       <c r="H24" t="s">
         <v>21</v>
       </c>
+      <c r="I24" t="s">
+        <v>28</v>
+      </c>
       <c r="J24" t="s">
         <v>25</v>
       </c>
       <c r="K24" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="L24" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D25">
         <v>10</v>
       </c>
@@ -3429,18 +4822,31 @@
       </c>
       <c r="I25">
         <f>(1/$L$23)*R7/($K$23*$I$23*H25*Table4[[#This Row],[Energy]])</f>
-        <v>8.8468372461033294E-31</v>
+        <v>1.4904080857349508E-26</v>
       </c>
       <c r="J25">
-        <f>1000*I25/(1E-28)</f>
-        <v>8.8468372461033304</v>
+        <f>I25/(1E-26)</f>
+        <v>1.4904080857349506</v>
       </c>
       <c r="K25">
-        <f>1000*SQRT(((I25*Table4[[#This Row],[Energy]])*M7)^2 / (Table4[[#This Row],[Energy]]^4))/1E-25</f>
-        <v>3.0407681286844026</v>
+        <f>SQRT(((I25*Table4[[#This Row],[Energy]])*M7)^2/(Table4[[#This Row],[Energy]]^4))/1E-25</f>
+        <v>51.22718187036304</v>
+      </c>
+      <c r="L25">
+        <f>SQRT((R7^2*H25^4*Table4[[#This Row],[EnergyErr]]^2+Table4[[#This Row],[Energy]]^2*(H25^4*Q26+R7^2*Table4[[#This Row],[EnergyErr]]^2*H25^2*0.2^2))/($L$23^2*Table4[[#This Row],[Energy]]^4*H25^4*$I$23^2*$K$23^2*H25^2))/1E-26</f>
+        <v>0.13864361043291312</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>30</v>
+      </c>
+      <c r="R25" t="s">
+        <v>33</v>
+      </c>
+      <c r="S25" t="s">
+        <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D26">
         <v>20</v>
       </c>
@@ -3449,7 +4855,7 @@
         <v>0.59436813200000005</v>
       </c>
       <c r="F26">
-        <f t="shared" ref="F26:F36" si="4">0.0000978*(E8)</f>
+        <f t="shared" ref="F26:F36" si="5">0.0000978*(E8)</f>
         <v>2.1080203200000004E-3</v>
       </c>
       <c r="H26">
@@ -3457,27 +4863,43 @@
       </c>
       <c r="I26">
         <f>(1/$L$23)*R8/($K$23*$I$23*H26*Table4[[#This Row],[Energy]])</f>
-        <v>8.683957826907454E-31</v>
+        <v>1.4629681321542212E-26</v>
       </c>
       <c r="J26">
-        <f t="shared" ref="J26:J36" si="5">1000*I26/(1E-28)</f>
-        <v>8.683957826907454</v>
+        <f t="shared" ref="J26:J36" si="6">I26/(1E-26)</f>
+        <v>1.4629681321542212</v>
       </c>
       <c r="K26">
-        <f>1000*SQRT(((I26*Table4[[#This Row],[Energy]])*M8)^2 / (Table4[[#This Row],[Energy]]^4))/1E-25</f>
-        <v>3.6349221155018201</v>
+        <f>SQRT(((I26*Table4[[#This Row],[Energy]])*M8)^2/(Table4[[#This Row],[Energy]]^4))/1E-25</f>
+        <v>61.236769268553026</v>
+      </c>
+      <c r="L26">
+        <f>SQRT((R8^2*H26^4*Table4[[#This Row],[EnergyErr]]^2+Table4[[#This Row],[Energy]]^2*(H26^4*Q27+R8^2*Table4[[#This Row],[EnergyErr]]^2*H26^2*0.2^2))/($L$23^2*Table4[[#This Row],[Energy]]^4*H26^4*$I$23^2*$K$23^2*H26^2))/1E-26</f>
+        <v>0.22296588944999363</v>
+      </c>
+      <c r="Q26">
+        <f>25*SQRT(PI()/2)*SQRT((M7^2*K7^2+J7^2*N7^2)/P7^2)/1024</f>
+        <v>0.21653570808358094</v>
+      </c>
+      <c r="R26">
+        <f>100*(SQRT(Q26/($L$23*E25^2*$I$23^2*$K$23^2*H25^2))/1E-26)/L25</f>
+        <v>39.383410159699096</v>
+      </c>
+      <c r="S26">
+        <f>100-R26</f>
+        <v>60.616589840300904</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D27">
         <v>30</v>
       </c>
       <c r="E27">
-        <f t="shared" ref="E26:E36" si="6">0.0000978*(D9)-0.0247</f>
+        <f t="shared" ref="E27:E36" si="7">0.0000978*(D9)-0.0247</f>
         <v>0.53855073800000008</v>
       </c>
       <c r="F27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.2218547400000002E-3</v>
       </c>
       <c r="H27">
@@ -3485,27 +4907,43 @@
       </c>
       <c r="I27">
         <f>(1/$L$23)*R9/($K$23*$I$23*H27*Table4[[#This Row],[Energy]])</f>
-        <v>7.474306296620203E-31</v>
+        <v>1.2591806800389616E-26</v>
       </c>
       <c r="J27">
-        <f t="shared" si="5"/>
-        <v>7.4743062966202034</v>
+        <f t="shared" si="6"/>
+        <v>1.2591806800389616</v>
       </c>
       <c r="K27">
-        <f>1000*SQRT(((I27*Table4[[#This Row],[Energy]])*M9)^2 / (Table4[[#This Row],[Energy]]^4))/1E-25</f>
-        <v>4.5170534523730943</v>
+        <f>SQRT(((I27*Table4[[#This Row],[Energy]])*M9)^2/(Table4[[#This Row],[Energy]]^4))/1E-25</f>
+        <v>76.097850585858964</v>
+      </c>
+      <c r="L27">
+        <f>SQRT((R9^2*H27^4*Table4[[#This Row],[EnergyErr]]^2+Table4[[#This Row],[Energy]]^2*(H27^4*Q28+R9^2*Table4[[#This Row],[EnergyErr]]^2*H27^2*0.2^2))/($L$23^2*Table4[[#This Row],[Energy]]^4*H27^4*$I$23^2*$K$23^2*H27^2))/1E-26</f>
+        <v>0.19706271721777735</v>
+      </c>
+      <c r="Q27">
+        <f t="shared" ref="Q27:Q36" si="8">25*SQRT(PI()/2)*SQRT((M8^2*K8^2+J8^2*N8^2)/P8^2)/1024</f>
+        <v>0.53405236070317597</v>
+      </c>
+      <c r="R27">
+        <f t="shared" ref="R27:R37" si="9">100*(SQRT(Q27/($L$23*E26^2*$I$23^2*$K$23^2*H26^2))/1E-26)/L26</f>
+        <v>39.376395751965006</v>
+      </c>
+      <c r="S27">
+        <f t="shared" ref="S27:S37" si="10">100-R27</f>
+        <v>60.623604248034994</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D28">
         <v>40</v>
       </c>
       <c r="E28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.47844285800000003</v>
       </c>
       <c r="F28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.3322807200000006E-3</v>
       </c>
       <c r="H28">
@@ -3513,27 +4951,43 @@
       </c>
       <c r="I28">
         <f>(1/$L$23)*R10/($K$23*$I$23*H28*Table4[[#This Row],[Energy]])</f>
-        <v>4.8666502748814833E-31</v>
+        <v>8.1987434812620344E-27</v>
       </c>
       <c r="J28">
-        <f t="shared" si="5"/>
-        <v>4.8666502748814837</v>
+        <f t="shared" si="6"/>
+        <v>0.81987434812620341</v>
       </c>
       <c r="K28">
-        <f>1000*SQRT(((I28*Table4[[#This Row],[Energy]])*M10)^2 / (Table4[[#This Row],[Energy]]^4))/1E-25</f>
-        <v>2.5582209529663267</v>
+        <f>SQRT(((I28*Table4[[#This Row],[Energy]])*M10)^2/(Table4[[#This Row],[Energy]]^4))/1E-25</f>
+        <v>43.097810972807984</v>
+      </c>
+      <c r="L28">
+        <f>SQRT((R10^2*H28^4*Table4[[#This Row],[EnergyErr]]^2+Table4[[#This Row],[Energy]]^2*(H28^4*Q29+R10^2*Table4[[#This Row],[EnergyErr]]^2*H28^2*0.2^2))/($L$23^2*Table4[[#This Row],[Energy]]^4*H28^4*$I$23^2*$K$23^2*H28^2))/1E-26</f>
+        <v>0.19225556943928462</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" si="8"/>
+        <v>0.43266273313983716</v>
+      </c>
+      <c r="R28">
+        <f t="shared" si="9"/>
+        <v>39.357670839589197</v>
+      </c>
+      <c r="S28">
+        <f t="shared" si="10"/>
+        <v>60.642329160410803</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D29">
         <v>50</v>
       </c>
       <c r="E29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.43234678399999998</v>
       </c>
       <c r="F29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.5780814600000006E-3</v>
       </c>
       <c r="H29">
@@ -3541,27 +4995,43 @@
       </c>
       <c r="I29">
         <f>(1/$L$23)*R11/($K$23*$I$23*H29*Table4[[#This Row],[Energy]])</f>
-        <v>5.2751612992158058E-31</v>
+        <v>8.8869534221060507E-27</v>
       </c>
       <c r="J29">
-        <f t="shared" si="5"/>
-        <v>5.2751612992158057</v>
+        <f t="shared" si="6"/>
+        <v>0.88869534221060509</v>
       </c>
       <c r="K29">
-        <f>1000*SQRT(((I29*Table4[[#This Row],[Energy]])*M11)^2 / (Table4[[#This Row],[Energy]]^4))/1E-25</f>
-        <v>3.4966276634297007</v>
+        <f>SQRT(((I29*Table4[[#This Row],[Energy]])*M11)^2/(Table4[[#This Row],[Energy]]^4))/1E-25</f>
+        <v>58.906951686892896</v>
+      </c>
+      <c r="L29">
+        <f>SQRT((R11^2*H29^4*Table4[[#This Row],[EnergyErr]]^2+Table4[[#This Row],[Energy]]^2*(H29^4*Q30+R11^2*Table4[[#This Row],[EnergyErr]]^2*H29^2*0.2^2))/($L$23^2*Table4[[#This Row],[Energy]]^4*H29^4*$I$23^2*$K$23^2*H29^2))/1E-26</f>
+        <v>0.1886249881086236</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" si="8"/>
+        <v>0.38668031517233775</v>
+      </c>
+      <c r="R29">
+        <f t="shared" si="9"/>
+        <v>39.369923294033882</v>
+      </c>
+      <c r="S29">
+        <f t="shared" si="10"/>
+        <v>60.630076705966118</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D30">
         <v>60</v>
       </c>
       <c r="E30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.39007566800000004</v>
       </c>
       <c r="F30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.8178088200000004E-3</v>
       </c>
       <c r="H30">
@@ -3569,27 +5039,43 @@
       </c>
       <c r="I30">
         <f>(1/$L$23)*R12/($K$23*$I$23*H30*Table4[[#This Row],[Energy]])</f>
-        <v>4.5985787343404505E-31</v>
+        <v>7.747128988462634E-27</v>
       </c>
       <c r="J30">
-        <f t="shared" si="5"/>
-        <v>4.5985787343404514</v>
+        <f t="shared" si="6"/>
+        <v>0.77471289884626338</v>
       </c>
       <c r="K30">
-        <f>1000*SQRT(((I30*Table4[[#This Row],[Energy]])*M12)^2 / (Table4[[#This Row],[Energy]]^4))/1E-25</f>
-        <v>3.0112490023668461</v>
+        <f>SQRT(((I30*Table4[[#This Row],[Energy]])*M12)^2/(Table4[[#This Row],[Energy]]^4))/1E-25</f>
+        <v>50.729879350562577</v>
+      </c>
+      <c r="L30">
+        <f>SQRT((R12^2*H30^4*Table4[[#This Row],[EnergyErr]]^2+Table4[[#This Row],[Energy]]^2*(H30^4*Q31+R12^2*Table4[[#This Row],[EnergyErr]]^2*H30^2*0.2^2))/($L$23^2*Table4[[#This Row],[Energy]]^4*H30^4*$I$23^2*$K$23^2*H30^2))/1E-26</f>
+        <v>0.23177695429664308</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="8"/>
+        <v>0.36969005290028328</v>
+      </c>
+      <c r="R30">
+        <f t="shared" si="9"/>
+        <v>39.357259652027373</v>
+      </c>
+      <c r="S30">
+        <f t="shared" si="10"/>
+        <v>60.642740347972627</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D31">
         <v>70</v>
       </c>
       <c r="E31">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.341972738</v>
       </c>
       <c r="F31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.0841914599999999E-3</v>
       </c>
       <c r="H31">
@@ -3597,27 +5083,43 @@
       </c>
       <c r="I31">
         <f>(1/$L$23)*R13/($K$23*$I$23*H31*Table4[[#This Row],[Energy]])</f>
-        <v>3.4815172498278647E-31</v>
+        <v>5.8652389723283869E-27</v>
       </c>
       <c r="J31">
-        <f t="shared" si="5"/>
-        <v>3.4815172498278648</v>
+        <f t="shared" si="6"/>
+        <v>0.58652389723283871</v>
       </c>
       <c r="K31">
-        <f>1000*SQRT(((I31*Table4[[#This Row],[Energy]])*M13)^2 / (Table4[[#This Row],[Energy]]^4))/1E-25</f>
-        <v>2.1533170094719414</v>
+        <f>SQRT(((I31*Table4[[#This Row],[Energy]])*M13)^2/(Table4[[#This Row],[Energy]]^4))/1E-25</f>
+        <v>36.276479297515728</v>
+      </c>
+      <c r="L31">
+        <f>SQRT((R13^2*H31^4*Table4[[#This Row],[EnergyErr]]^2+Table4[[#This Row],[Energy]]^2*(H31^4*Q32+R13^2*Table4[[#This Row],[EnergyErr]]^2*H31^2*0.2^2))/($L$23^2*Table4[[#This Row],[Energy]]^4*H31^4*$I$23^2*$K$23^2*H31^2))/1E-26</f>
+        <v>0.17772508403410603</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" si="8"/>
+        <v>0.49011466198983411</v>
+      </c>
+      <c r="R31">
+        <f t="shared" si="9"/>
+        <v>39.366435210210497</v>
+      </c>
+      <c r="S31">
+        <f t="shared" si="10"/>
+        <v>60.633564789789503</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D32">
         <v>80</v>
       </c>
       <c r="E32">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.30590996599999998</v>
       </c>
       <c r="F32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2339132600000002E-3</v>
       </c>
       <c r="H32">
@@ -3625,27 +5127,43 @@
       </c>
       <c r="I32">
         <f>(1/$L$23)*R14/($K$23*$I$23*H32*Table4[[#This Row],[Energy]])</f>
-        <v>3.9183468599842185E-31</v>
+        <v>6.6011566398001589E-27</v>
       </c>
       <c r="J32">
-        <f t="shared" si="5"/>
-        <v>3.9183468599842191</v>
+        <f t="shared" si="6"/>
+        <v>0.66011566398001587</v>
       </c>
       <c r="K32">
-        <f>1000*SQRT(((I32*Table4[[#This Row],[Energy]])*M14)^2 / (Table4[[#This Row],[Energy]]^4))/1E-25</f>
-        <v>2.3467046124862398</v>
+        <f>SQRT(((I32*Table4[[#This Row],[Energy]])*M14)^2/(Table4[[#This Row],[Energy]]^4))/1E-25</f>
+        <v>39.534439619328623</v>
+      </c>
+      <c r="L32">
+        <f>SQRT((R14^2*H32^4*Table4[[#This Row],[EnergyErr]]^2+Table4[[#This Row],[Energy]]^2*(H32^4*Q33+R14^2*Table4[[#This Row],[EnergyErr]]^2*H32^2*0.2^2))/($L$23^2*Table4[[#This Row],[Energy]]^4*H32^4*$I$23^2*$K$23^2*H32^2))/1E-26</f>
+        <v>0.12986303721844897</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" si="8"/>
+        <v>0.26181941453164514</v>
+      </c>
+      <c r="R32">
+        <f t="shared" si="9"/>
+        <v>39.370226996614868</v>
+      </c>
+      <c r="S32">
+        <f t="shared" si="10"/>
+        <v>60.629773003385132</v>
       </c>
     </row>
-    <row r="33" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D33">
         <v>90</v>
       </c>
       <c r="E33">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.27188339000000006</v>
       </c>
       <c r="F33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.3937086800000001E-3</v>
       </c>
       <c r="H33">
@@ -3653,27 +5171,43 @@
       </c>
       <c r="I33">
         <f>(1/$L$23)*R15/($K$23*$I$23*H33*Table4[[#This Row],[Energy]])</f>
-        <v>2.9556034951330276E-31</v>
+        <v>4.9792431180001565E-27</v>
       </c>
       <c r="J33">
-        <f t="shared" si="5"/>
-        <v>2.9556034951330274</v>
+        <f t="shared" si="6"/>
+        <v>0.49792431180001562</v>
       </c>
       <c r="K33">
-        <f>1000*SQRT(((I33*Table4[[#This Row],[Energy]])*M15)^2 / (Table4[[#This Row],[Energy]]^4))/1E-25</f>
-        <v>1.6979180298760712</v>
+        <f>SQRT(((I33*Table4[[#This Row],[Energy]])*M15)^2/(Table4[[#This Row],[Energy]]^4))/1E-25</f>
+        <v>28.604468356836524</v>
+      </c>
+      <c r="L33">
+        <f>SQRT((R15^2*H33^4*Table4[[#This Row],[EnergyErr]]^2+Table4[[#This Row],[Energy]]^2*(H33^4*Q34+R15^2*Table4[[#This Row],[EnergyErr]]^2*H33^2*0.2^2))/($L$23^2*Table4[[#This Row],[Energy]]^4*H33^4*$I$23^2*$K$23^2*H33^2))/1E-26</f>
+        <v>0.13507038428660223</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" si="8"/>
+        <v>0.13689200576453134</v>
+      </c>
+      <c r="R33">
+        <f t="shared" si="9"/>
+        <v>39.379525623080269</v>
+      </c>
+      <c r="S33">
+        <f t="shared" si="10"/>
+        <v>60.620474376919731</v>
       </c>
     </row>
-    <row r="34" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D34">
         <v>-10</v>
       </c>
       <c r="E34">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.62802893599999998</v>
       </c>
       <c r="F34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.4671517000000001E-3</v>
       </c>
       <c r="H34">
@@ -3681,27 +5215,43 @@
       </c>
       <c r="I34">
         <f>(1/$L$23)*R16/($K$23*$I$23*H34*Table4[[#This Row],[Energy]])</f>
-        <v>5.8984545283692428E-31</v>
+        <v>9.9370024313418643E-27</v>
       </c>
       <c r="J34">
-        <f t="shared" si="5"/>
-        <v>5.8984545283692427</v>
+        <f t="shared" si="6"/>
+        <v>0.99370024313418637</v>
       </c>
       <c r="K34">
-        <f>1000*SQRT(((I34*Table4[[#This Row],[Energy]])*M16)^2 / (Table4[[#This Row],[Energy]]^4))/1E-25</f>
-        <v>2.2556792257075888</v>
+        <f>SQRT(((I34*Table4[[#This Row],[Energy]])*M16)^2/(Table4[[#This Row],[Energy]]^4))/1E-25</f>
+        <v>38.000954050553098</v>
+      </c>
+      <c r="L34">
+        <f>SQRT((R16^2*H34^4*Table4[[#This Row],[EnergyErr]]^2+Table4[[#This Row],[Energy]]^2*(H34^4*Q35+R16^2*Table4[[#This Row],[EnergyErr]]^2*H34^2*0.2^2))/($L$23^2*Table4[[#This Row],[Energy]]^4*H34^4*$I$23^2*$K$23^2*H34^2))/1E-26</f>
+        <v>0.17658449624656516</v>
+      </c>
+      <c r="Q34">
+        <f t="shared" si="8"/>
+        <v>0.12786263431138362</v>
+      </c>
+      <c r="R34">
+        <f t="shared" si="9"/>
+        <v>39.380794645334262</v>
+      </c>
+      <c r="S34">
+        <f t="shared" si="10"/>
+        <v>60.619205354665738</v>
       </c>
     </row>
-    <row r="35" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D35">
         <v>-20</v>
       </c>
       <c r="E35">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.59241506600000005</v>
       </c>
       <c r="F35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.7717350200000001E-3</v>
       </c>
       <c r="H35">
@@ -3709,27 +5259,43 @@
       </c>
       <c r="I35">
         <f>(1/$L$23)*R17/($K$23*$I$23*H35*Table4[[#This Row],[Energy]])</f>
-        <v>8.4641849857139268E-31</v>
+        <v>1.4259434632891927E-26</v>
       </c>
       <c r="J35">
-        <f t="shared" si="5"/>
-        <v>8.4641849857139277</v>
+        <f t="shared" si="6"/>
+        <v>1.4259434632891927</v>
       </c>
       <c r="K35">
-        <f>1000*SQRT(((I35*Table4[[#This Row],[Energy]])*M17)^2 / (Table4[[#This Row],[Energy]]^4))/1E-25</f>
-        <v>3.14112718583225</v>
+        <f>SQRT(((I35*Table4[[#This Row],[Energy]])*M17)^2/(Table4[[#This Row],[Energy]]^4))/1E-25</f>
+        <v>52.917909823064647</v>
+      </c>
+      <c r="L35">
+        <f>SQRT((R17^2*H35^4*Table4[[#This Row],[EnergyErr]]^2+Table4[[#This Row],[Energy]]^2*(H35^4*Q36+R17^2*Table4[[#This Row],[EnergyErr]]^2*H35^2*0.2^2))/($L$23^2*Table4[[#This Row],[Energy]]^4*H35^4*$I$23^2*$K$23^2*H35^2))/1E-26</f>
+        <v>0.21784691183748625</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" si="8"/>
+        <v>0.35259794849095966</v>
+      </c>
+      <c r="R35">
+        <f t="shared" si="9"/>
+        <v>39.377381749086815</v>
+      </c>
+      <c r="S35">
+        <f t="shared" si="10"/>
+        <v>60.622618250913185</v>
       </c>
     </row>
-    <row r="36" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D36">
         <v>-30</v>
       </c>
       <c r="E36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.54427008199999993</v>
       </c>
       <c r="F36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.6491477199999999E-3</v>
       </c>
       <c r="H36">
@@ -3737,15 +5303,45 @@
       </c>
       <c r="I36">
         <f>(1/$L$23)*R18/($K$23*$I$23*H36*Table4[[#This Row],[Energy]])</f>
-        <v>7.3774606491882665E-31</v>
+        <v>1.2428652972659407E-26</v>
       </c>
       <c r="J36">
-        <f t="shared" si="5"/>
-        <v>7.3774606491882659</v>
+        <f t="shared" si="6"/>
+        <v>1.2428652972659406</v>
       </c>
       <c r="K36">
-        <f>1000*SQRT(((I36*Table4[[#This Row],[Energy]])*M18)^2 / (Table4[[#This Row],[Energy]]^4))/1E-25</f>
-        <v>3.7691773819009606</v>
+        <f>SQRT(((I36*Table4[[#This Row],[Energy]])*M18)^2/(Table4[[#This Row],[Energy]]^4))/1E-25</f>
+        <v>63.498539537717996</v>
+      </c>
+      <c r="L36">
+        <f>SQRT((R18^2*H36^4*Table4[[#This Row],[EnergyErr]]^2+Table4[[#This Row],[Energy]]^2*(H36^4*Q37+R18^2*Table4[[#This Row],[EnergyErr]]^2*H36^2*0.2^2))/($L$23^2*Table4[[#This Row],[Energy]]^4*H36^4*$I$23^2*$K$23^2*H36^2))/1E-26</f>
+        <v>0.23009019627604299</v>
+      </c>
+      <c r="Q36">
+        <f t="shared" si="8"/>
+        <v>0.50655312385973605</v>
+      </c>
+      <c r="R36">
+        <f t="shared" si="9"/>
+        <v>39.379752422023998</v>
+      </c>
+      <c r="S36">
+        <f t="shared" si="10"/>
+        <v>60.620247577976002</v>
+      </c>
+    </row>
+    <row r="37" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="Q37">
+        <f t="shared" ref="Q37" si="11">25*SQRT(PI()/2)*SQRT((M18^2*K18^2+J18^2*N18^2)/P18^2)/1024</f>
+        <v>0.53802542544405896</v>
+      </c>
+      <c r="R37">
+        <f t="shared" si="9"/>
+        <v>39.373487612387983</v>
+      </c>
+      <c r="S37">
+        <f t="shared" si="10"/>
+        <v>60.626512387612017</v>
       </c>
     </row>
   </sheetData>

</xml_diff>